<commit_message>
Added Prsn_time_yrs to codebook and dictionary
</commit_message>
<xml_diff>
--- a/JohnGroupB_datadictionary.xlsx
+++ b/JohnGroupB_datadictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Desktop\Epidem207_JohnB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0FFC45AE-DFC5-4365-947E-87ADB8CCEB96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348A6414-40EE-4AF7-B632-F113626C2240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-118" yWindow="-118" windowWidth="33749" windowHeight="18471" xr2:uid="{6C4BF825-8825-4C8C-BB19-5DDDEC53018B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="112">
   <si>
     <t>Variable Name</t>
   </si>
@@ -195,12 +195,6 @@
     <t>prsn_time</t>
   </si>
   <si>
-    <t>Person-Time (Continuous)</t>
-  </si>
-  <si>
-    <t>Amount of person-time contributed to the study by the subject. Tentative unit: Person-days</t>
-  </si>
-  <si>
     <t>151-8035</t>
   </si>
   <si>
@@ -291,9 +285,6 @@
     <t>13</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -361,6 +352,24 @@
   </si>
   <si>
     <t>1= Low to Moderate Alcohol, Never Smoker || 2= Low to Moderate Alcohol, Former Daily Smoker || 3= Low to Moderate Alcohol, Current Smoker (&lt;=-19 cig/day) || 4= Low to Moderate Alcohol, Current Smoker (&gt;19 cig/day) || 5= Moderate to High Alcohol, Never Smoker || 6= Moderate to High Alcohol, Former Daily Smoker || 7= Moderate to High Alcohol, Current Smoker (&lt;=19 cig/day) || 8= Moderate to High Alcohol, Current Smoker (&gt;19 cig/day) || 9= Very High Alcohol, Not Current Smoker || 10= Very High Alcohol, Current Smoker (&lt;=19 cig/day) || 11= Very High Alcohol, Current Smoker (&gt;19 cig/day) || 12= Extremely High Alcohol, Not Current Smoker || 13= Extremely High Alcohol, Current Smoker || 14= Abstinent at Baseline, Good Health  || 15= Abstinent at Baseline, History of Alcohol/Drug Dependence || 16= Abstinent at Baseline, History of Risk Drinking || 17= Abstinent at Baseline, Tried to Cut Down or Stop  || 18= Abstinent at Baseline, Current Daily Smoker (&gt;19 cig/day) || 19= Abstinent at Baseline, Current Daily Smoker (&lt;=19 cig/day) || 20= Abstinent at Baseline, Former Smoker || 21= Abstinent at Baseline, Poor Health</t>
+  </si>
+  <si>
+    <t>prsn_time_yrs</t>
+  </si>
+  <si>
+    <t>Amount of person-time contributed to the study by the subject. Unit: Person-days</t>
+  </si>
+  <si>
+    <t>Amount of person-time contributed to the study by the subject. Unit: Person-years</t>
+  </si>
+  <si>
+    <t>0-22</t>
+  </si>
+  <si>
+    <t>Person-Time (Continuous, years)</t>
+  </si>
+  <si>
+    <t>Person-Time (Continuous, days)</t>
   </si>
 </sst>
 </file>
@@ -409,7 +418,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -461,29 +470,15 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -506,9 +501,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -522,9 +514,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -552,16 +541,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -572,33 +552,31 @@
     <xf numFmtId="20" fontId="1" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="1" fillId="3" borderId="4" xfId="2" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="3" borderId="2" xfId="2" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
@@ -915,10 +893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F21591B-10C8-4FF7-A2B4-B95B76AA0644}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -927,475 +905,504 @@
     <col min="2" max="2" width="9.5546875" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" customWidth="1"/>
     <col min="4" max="4" width="30.109375" customWidth="1"/>
-    <col min="5" max="5" width="51.109375" style="25" customWidth="1"/>
+    <col min="5" max="5" width="51.109375" style="22" customWidth="1"/>
     <col min="6" max="6" width="20.5546875" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
     <col min="8" max="8" width="15.44140625" customWidth="1"/>
     <col min="9" max="9" width="71.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="31" customFormat="1" ht="42.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:9" s="25" customFormat="1" ht="42.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C3" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="30" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="13" t="s">
+      <c r="C6" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="9" customFormat="1" ht="30.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="29" customFormat="1" ht="30.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="30">
+        <v>8</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="I12" s="29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="5" customFormat="1" ht="121.1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="3">
+        <v>8</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H13" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="29" customFormat="1" ht="211.45" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="30">
+        <v>8</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="H14" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="I14" s="29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="5" customFormat="1" ht="195.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="12" t="s">
+      <c r="C15" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="G15" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" s="21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="12" t="s">
+      <c r="D16" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="30.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="14" t="s">
+      <c r="G16" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="35" customFormat="1" ht="30.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="19" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="30.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="32" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="30.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="I10" s="9" t="s">
+      <c r="G17" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="I17" s="28" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" s="10" customFormat="1" ht="30.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" s="10" customFormat="1" ht="121.1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="35" t="s">
-        <v>101</v>
-      </c>
-      <c r="B12" s="36" t="s">
-        <v>89</v>
-      </c>
-      <c r="C12" s="36">
-        <v>8</v>
-      </c>
-      <c r="D12" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="E12" s="41" t="s">
-        <v>94</v>
-      </c>
-      <c r="F12" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="36" t="s">
-        <v>103</v>
-      </c>
-      <c r="H12" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="I12" s="40" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="10" customFormat="1" ht="211.45" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="B13" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="C13" s="21">
-        <v>8</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="E13" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="F13" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="33" t="s">
-        <v>104</v>
-      </c>
-      <c r="H13" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="I13" s="34" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" s="10" customFormat="1" ht="195.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="I14" s="16" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="H15" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" s="2" customFormat="1" ht="30.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="C16" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="D16" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="E16" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="F16" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="H16" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="I16" s="29" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>